<commit_message>
window column data added
</commit_message>
<xml_diff>
--- a/cuadro_columnas.xlsx
+++ b/cuadro_columnas.xlsx
@@ -936,6 +936,36 @@
           <t>Detalle</t>
         </is>
       </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>DC-11</t>
+        </is>
+      </c>
+      <c r="Q28" t="inlineStr">
+        <is>
+          <t>DC-11</t>
+        </is>
+      </c>
+      <c r="R28" t="inlineStr">
+        <is>
+          <t>DC-11</t>
+        </is>
+      </c>
+      <c r="S28" t="inlineStr">
+        <is>
+          <t>DC-11</t>
+        </is>
+      </c>
+      <c r="U28" t="inlineStr">
+        <is>
+          <t>DC-11</t>
+        </is>
+      </c>
+      <c r="V28" t="inlineStr">
+        <is>
+          <t>DC-11</t>
+        </is>
+      </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
@@ -1214,6 +1244,76 @@
           <t>Detalle</t>
         </is>
       </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>DC-11</t>
+        </is>
+      </c>
+      <c r="G37" t="inlineStr">
+        <is>
+          <t>DC-11</t>
+        </is>
+      </c>
+      <c r="H37" t="inlineStr">
+        <is>
+          <t>DC-11</t>
+        </is>
+      </c>
+      <c r="K37" t="inlineStr">
+        <is>
+          <t>DC-5</t>
+        </is>
+      </c>
+      <c r="L37" t="inlineStr">
+        <is>
+          <t>DC-5</t>
+        </is>
+      </c>
+      <c r="O37" t="inlineStr">
+        <is>
+          <t>DC-11</t>
+        </is>
+      </c>
+      <c r="P37" t="inlineStr">
+        <is>
+          <t>DC-11</t>
+        </is>
+      </c>
+      <c r="Q37" t="inlineStr">
+        <is>
+          <t>DC-11</t>
+        </is>
+      </c>
+      <c r="R37" t="inlineStr">
+        <is>
+          <t>DC-11</t>
+        </is>
+      </c>
+      <c r="S37" t="inlineStr">
+        <is>
+          <t>DC-11</t>
+        </is>
+      </c>
+      <c r="T37" t="inlineStr">
+        <is>
+          <t>DC-11</t>
+        </is>
+      </c>
+      <c r="U37" t="inlineStr">
+        <is>
+          <t>DC-11</t>
+        </is>
+      </c>
+      <c r="V37" t="inlineStr">
+        <is>
+          <t>DC-11</t>
+        </is>
+      </c>
+      <c r="W37" t="inlineStr">
+        <is>
+          <t>DC-11</t>
+        </is>
+      </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
@@ -1492,6 +1592,76 @@
           <t>Detalle</t>
         </is>
       </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>DC-11</t>
+        </is>
+      </c>
+      <c r="G46" t="inlineStr">
+        <is>
+          <t>DC-11</t>
+        </is>
+      </c>
+      <c r="H46" t="inlineStr">
+        <is>
+          <t>DC-11</t>
+        </is>
+      </c>
+      <c r="K46" t="inlineStr">
+        <is>
+          <t>DC-5</t>
+        </is>
+      </c>
+      <c r="L46" t="inlineStr">
+        <is>
+          <t>DC-5</t>
+        </is>
+      </c>
+      <c r="O46" t="inlineStr">
+        <is>
+          <t>DC-11</t>
+        </is>
+      </c>
+      <c r="P46" t="inlineStr">
+        <is>
+          <t>DC-11</t>
+        </is>
+      </c>
+      <c r="Q46" t="inlineStr">
+        <is>
+          <t>DC-11</t>
+        </is>
+      </c>
+      <c r="R46" t="inlineStr">
+        <is>
+          <t>DC-11</t>
+        </is>
+      </c>
+      <c r="S46" t="inlineStr">
+        <is>
+          <t>DC-11</t>
+        </is>
+      </c>
+      <c r="T46" t="inlineStr">
+        <is>
+          <t>DC-11</t>
+        </is>
+      </c>
+      <c r="U46" t="inlineStr">
+        <is>
+          <t>DC-11</t>
+        </is>
+      </c>
+      <c r="V46" t="inlineStr">
+        <is>
+          <t>DC-11</t>
+        </is>
+      </c>
+      <c r="W46" t="inlineStr">
+        <is>
+          <t>DC-11</t>
+        </is>
+      </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
@@ -1770,6 +1940,76 @@
           <t>Detalle</t>
         </is>
       </c>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t>DC-11</t>
+        </is>
+      </c>
+      <c r="G55" t="inlineStr">
+        <is>
+          <t>DC-11</t>
+        </is>
+      </c>
+      <c r="H55" t="inlineStr">
+        <is>
+          <t>DC-11</t>
+        </is>
+      </c>
+      <c r="K55" t="inlineStr">
+        <is>
+          <t>DC-5</t>
+        </is>
+      </c>
+      <c r="L55" t="inlineStr">
+        <is>
+          <t>DC-5</t>
+        </is>
+      </c>
+      <c r="O55" t="inlineStr">
+        <is>
+          <t>DC-11</t>
+        </is>
+      </c>
+      <c r="P55" t="inlineStr">
+        <is>
+          <t>DC-11</t>
+        </is>
+      </c>
+      <c r="Q55" t="inlineStr">
+        <is>
+          <t>DC-11</t>
+        </is>
+      </c>
+      <c r="R55" t="inlineStr">
+        <is>
+          <t>DC-11</t>
+        </is>
+      </c>
+      <c r="S55" t="inlineStr">
+        <is>
+          <t>DC-11</t>
+        </is>
+      </c>
+      <c r="T55" t="inlineStr">
+        <is>
+          <t>DC-11</t>
+        </is>
+      </c>
+      <c r="U55" t="inlineStr">
+        <is>
+          <t>DC-11</t>
+        </is>
+      </c>
+      <c r="V55" t="inlineStr">
+        <is>
+          <t>DC-11</t>
+        </is>
+      </c>
+      <c r="W55" t="inlineStr">
+        <is>
+          <t>DC-11</t>
+        </is>
+      </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
@@ -2048,6 +2288,76 @@
           <t>Detalle</t>
         </is>
       </c>
+      <c r="C64" t="inlineStr">
+        <is>
+          <t>DC-11</t>
+        </is>
+      </c>
+      <c r="G64" t="inlineStr">
+        <is>
+          <t>DC-11</t>
+        </is>
+      </c>
+      <c r="H64" t="inlineStr">
+        <is>
+          <t>DC-11</t>
+        </is>
+      </c>
+      <c r="K64" t="inlineStr">
+        <is>
+          <t>DC-5</t>
+        </is>
+      </c>
+      <c r="L64" t="inlineStr">
+        <is>
+          <t>DC-5</t>
+        </is>
+      </c>
+      <c r="O64" t="inlineStr">
+        <is>
+          <t>DC-11</t>
+        </is>
+      </c>
+      <c r="P64" t="inlineStr">
+        <is>
+          <t>DC-11</t>
+        </is>
+      </c>
+      <c r="Q64" t="inlineStr">
+        <is>
+          <t>DC-11</t>
+        </is>
+      </c>
+      <c r="R64" t="inlineStr">
+        <is>
+          <t>DC-11</t>
+        </is>
+      </c>
+      <c r="S64" t="inlineStr">
+        <is>
+          <t>DC-11</t>
+        </is>
+      </c>
+      <c r="T64" t="inlineStr">
+        <is>
+          <t>DC-11</t>
+        </is>
+      </c>
+      <c r="U64" t="inlineStr">
+        <is>
+          <t>DC-11</t>
+        </is>
+      </c>
+      <c r="V64" t="inlineStr">
+        <is>
+          <t>DC-11</t>
+        </is>
+      </c>
+      <c r="W64" t="inlineStr">
+        <is>
+          <t>DC-11</t>
+        </is>
+      </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
@@ -2326,6 +2636,76 @@
           <t>Detalle</t>
         </is>
       </c>
+      <c r="C73" t="inlineStr">
+        <is>
+          <t>DC-11</t>
+        </is>
+      </c>
+      <c r="G73" t="inlineStr">
+        <is>
+          <t>DC-11</t>
+        </is>
+      </c>
+      <c r="H73" t="inlineStr">
+        <is>
+          <t>DC-11</t>
+        </is>
+      </c>
+      <c r="K73" t="inlineStr">
+        <is>
+          <t>DC-5</t>
+        </is>
+      </c>
+      <c r="L73" t="inlineStr">
+        <is>
+          <t>DC-5</t>
+        </is>
+      </c>
+      <c r="O73" t="inlineStr">
+        <is>
+          <t>DC-11</t>
+        </is>
+      </c>
+      <c r="P73" t="inlineStr">
+        <is>
+          <t>DC-11</t>
+        </is>
+      </c>
+      <c r="Q73" t="inlineStr">
+        <is>
+          <t>DC-11</t>
+        </is>
+      </c>
+      <c r="R73" t="inlineStr">
+        <is>
+          <t>DC-11</t>
+        </is>
+      </c>
+      <c r="S73" t="inlineStr">
+        <is>
+          <t>DC-11</t>
+        </is>
+      </c>
+      <c r="T73" t="inlineStr">
+        <is>
+          <t>DC-11</t>
+        </is>
+      </c>
+      <c r="U73" t="inlineStr">
+        <is>
+          <t>DC-11</t>
+        </is>
+      </c>
+      <c r="V73" t="inlineStr">
+        <is>
+          <t>DC-11</t>
+        </is>
+      </c>
+      <c r="W73" t="inlineStr">
+        <is>
+          <t>DC-11</t>
+        </is>
+      </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
@@ -2604,6 +2984,76 @@
           <t>Detalle</t>
         </is>
       </c>
+      <c r="C82" t="inlineStr">
+        <is>
+          <t>DC-11</t>
+        </is>
+      </c>
+      <c r="G82" t="inlineStr">
+        <is>
+          <t>DC-11</t>
+        </is>
+      </c>
+      <c r="H82" t="inlineStr">
+        <is>
+          <t>DC-11</t>
+        </is>
+      </c>
+      <c r="K82" t="inlineStr">
+        <is>
+          <t>DC-9</t>
+        </is>
+      </c>
+      <c r="L82" t="inlineStr">
+        <is>
+          <t>DC-9</t>
+        </is>
+      </c>
+      <c r="O82" t="inlineStr">
+        <is>
+          <t>DC-11</t>
+        </is>
+      </c>
+      <c r="P82" t="inlineStr">
+        <is>
+          <t>DC-11</t>
+        </is>
+      </c>
+      <c r="Q82" t="inlineStr">
+        <is>
+          <t>DC-11</t>
+        </is>
+      </c>
+      <c r="R82" t="inlineStr">
+        <is>
+          <t>DC-11</t>
+        </is>
+      </c>
+      <c r="S82" t="inlineStr">
+        <is>
+          <t>DC-11</t>
+        </is>
+      </c>
+      <c r="T82" t="inlineStr">
+        <is>
+          <t>DC-11</t>
+        </is>
+      </c>
+      <c r="U82" t="inlineStr">
+        <is>
+          <t>DC-11</t>
+        </is>
+      </c>
+      <c r="V82" t="inlineStr">
+        <is>
+          <t>DC-11</t>
+        </is>
+      </c>
+      <c r="W82" t="inlineStr">
+        <is>
+          <t>DC-11</t>
+        </is>
+      </c>
     </row>
     <row r="83">
       <c r="A83" t="inlineStr">
@@ -2882,6 +3332,76 @@
           <t>Detalle</t>
         </is>
       </c>
+      <c r="C91" t="inlineStr">
+        <is>
+          <t>DC-11</t>
+        </is>
+      </c>
+      <c r="G91" t="inlineStr">
+        <is>
+          <t>DC-11</t>
+        </is>
+      </c>
+      <c r="H91" t="inlineStr">
+        <is>
+          <t>DC-11</t>
+        </is>
+      </c>
+      <c r="K91" t="inlineStr">
+        <is>
+          <t>DC-9</t>
+        </is>
+      </c>
+      <c r="L91" t="inlineStr">
+        <is>
+          <t>DC-9</t>
+        </is>
+      </c>
+      <c r="O91" t="inlineStr">
+        <is>
+          <t>DC-11</t>
+        </is>
+      </c>
+      <c r="P91" t="inlineStr">
+        <is>
+          <t>DC-11</t>
+        </is>
+      </c>
+      <c r="Q91" t="inlineStr">
+        <is>
+          <t>DC-11</t>
+        </is>
+      </c>
+      <c r="R91" t="inlineStr">
+        <is>
+          <t>DC-11</t>
+        </is>
+      </c>
+      <c r="S91" t="inlineStr">
+        <is>
+          <t>DC-11</t>
+        </is>
+      </c>
+      <c r="T91" t="inlineStr">
+        <is>
+          <t>DC-11</t>
+        </is>
+      </c>
+      <c r="U91" t="inlineStr">
+        <is>
+          <t>DC-11</t>
+        </is>
+      </c>
+      <c r="V91" t="inlineStr">
+        <is>
+          <t>DC-11</t>
+        </is>
+      </c>
+      <c r="W91" t="inlineStr">
+        <is>
+          <t>DC-11</t>
+        </is>
+      </c>
     </row>
     <row r="92">
       <c r="A92" t="inlineStr">
@@ -3160,6 +3680,76 @@
           <t>Detalle</t>
         </is>
       </c>
+      <c r="C100" t="inlineStr">
+        <is>
+          <t>DC-11</t>
+        </is>
+      </c>
+      <c r="G100" t="inlineStr">
+        <is>
+          <t>DC-11</t>
+        </is>
+      </c>
+      <c r="H100" t="inlineStr">
+        <is>
+          <t>DC-11</t>
+        </is>
+      </c>
+      <c r="K100" t="inlineStr">
+        <is>
+          <t>DC-9</t>
+        </is>
+      </c>
+      <c r="L100" t="inlineStr">
+        <is>
+          <t>DC-9</t>
+        </is>
+      </c>
+      <c r="O100" t="inlineStr">
+        <is>
+          <t>DC-11</t>
+        </is>
+      </c>
+      <c r="P100" t="inlineStr">
+        <is>
+          <t>DC-11</t>
+        </is>
+      </c>
+      <c r="Q100" t="inlineStr">
+        <is>
+          <t>DC-11</t>
+        </is>
+      </c>
+      <c r="R100" t="inlineStr">
+        <is>
+          <t>DC-11</t>
+        </is>
+      </c>
+      <c r="S100" t="inlineStr">
+        <is>
+          <t>DC-11</t>
+        </is>
+      </c>
+      <c r="T100" t="inlineStr">
+        <is>
+          <t>DC-11</t>
+        </is>
+      </c>
+      <c r="U100" t="inlineStr">
+        <is>
+          <t>DC-11</t>
+        </is>
+      </c>
+      <c r="V100" t="inlineStr">
+        <is>
+          <t>DC-11</t>
+        </is>
+      </c>
+      <c r="W100" t="inlineStr">
+        <is>
+          <t>DC-11</t>
+        </is>
+      </c>
     </row>
     <row r="101">
       <c r="A101" t="inlineStr">
@@ -3438,6 +4028,76 @@
           <t>Detalle</t>
         </is>
       </c>
+      <c r="C109" t="inlineStr">
+        <is>
+          <t>DC-11</t>
+        </is>
+      </c>
+      <c r="G109" t="inlineStr">
+        <is>
+          <t>DC-11</t>
+        </is>
+      </c>
+      <c r="H109" t="inlineStr">
+        <is>
+          <t>DC-11</t>
+        </is>
+      </c>
+      <c r="K109" t="inlineStr">
+        <is>
+          <t>DC-9</t>
+        </is>
+      </c>
+      <c r="L109" t="inlineStr">
+        <is>
+          <t>DC-9</t>
+        </is>
+      </c>
+      <c r="O109" t="inlineStr">
+        <is>
+          <t>DC-11</t>
+        </is>
+      </c>
+      <c r="P109" t="inlineStr">
+        <is>
+          <t>DC-11</t>
+        </is>
+      </c>
+      <c r="Q109" t="inlineStr">
+        <is>
+          <t>DC-11</t>
+        </is>
+      </c>
+      <c r="R109" t="inlineStr">
+        <is>
+          <t>DC-11</t>
+        </is>
+      </c>
+      <c r="S109" t="inlineStr">
+        <is>
+          <t>DC-11</t>
+        </is>
+      </c>
+      <c r="T109" t="inlineStr">
+        <is>
+          <t>DC-11</t>
+        </is>
+      </c>
+      <c r="U109" t="inlineStr">
+        <is>
+          <t>DC-11</t>
+        </is>
+      </c>
+      <c r="V109" t="inlineStr">
+        <is>
+          <t>DC-11</t>
+        </is>
+      </c>
+      <c r="W109" t="inlineStr">
+        <is>
+          <t>DC-11</t>
+        </is>
+      </c>
     </row>
     <row r="110">
       <c r="A110" t="inlineStr">
@@ -3716,6 +4376,76 @@
           <t>Detalle</t>
         </is>
       </c>
+      <c r="C118" t="inlineStr">
+        <is>
+          <t>DC-11</t>
+        </is>
+      </c>
+      <c r="G118" t="inlineStr">
+        <is>
+          <t>DC-11</t>
+        </is>
+      </c>
+      <c r="H118" t="inlineStr">
+        <is>
+          <t>DC-11</t>
+        </is>
+      </c>
+      <c r="K118" t="inlineStr">
+        <is>
+          <t>DC-9</t>
+        </is>
+      </c>
+      <c r="L118" t="inlineStr">
+        <is>
+          <t>DC-9</t>
+        </is>
+      </c>
+      <c r="O118" t="inlineStr">
+        <is>
+          <t>DC-11</t>
+        </is>
+      </c>
+      <c r="P118" t="inlineStr">
+        <is>
+          <t>DC-11</t>
+        </is>
+      </c>
+      <c r="Q118" t="inlineStr">
+        <is>
+          <t>DC-11</t>
+        </is>
+      </c>
+      <c r="R118" t="inlineStr">
+        <is>
+          <t>DC-11</t>
+        </is>
+      </c>
+      <c r="S118" t="inlineStr">
+        <is>
+          <t>DC-11</t>
+        </is>
+      </c>
+      <c r="T118" t="inlineStr">
+        <is>
+          <t>DC-11</t>
+        </is>
+      </c>
+      <c r="U118" t="inlineStr">
+        <is>
+          <t>DC-11</t>
+        </is>
+      </c>
+      <c r="V118" t="inlineStr">
+        <is>
+          <t>DC-11</t>
+        </is>
+      </c>
+      <c r="W118" t="inlineStr">
+        <is>
+          <t>DC-11</t>
+        </is>
+      </c>
     </row>
     <row r="119">
       <c r="A119" t="inlineStr">
@@ -3994,6 +4724,76 @@
           <t>Detalle</t>
         </is>
       </c>
+      <c r="C127" t="inlineStr">
+        <is>
+          <t>DC-11</t>
+        </is>
+      </c>
+      <c r="G127" t="inlineStr">
+        <is>
+          <t>DC-11</t>
+        </is>
+      </c>
+      <c r="H127" t="inlineStr">
+        <is>
+          <t>DC-11</t>
+        </is>
+      </c>
+      <c r="K127" t="inlineStr">
+        <is>
+          <t>DC-9</t>
+        </is>
+      </c>
+      <c r="L127" t="inlineStr">
+        <is>
+          <t>DC-9</t>
+        </is>
+      </c>
+      <c r="O127" t="inlineStr">
+        <is>
+          <t>DC-11</t>
+        </is>
+      </c>
+      <c r="P127" t="inlineStr">
+        <is>
+          <t>DC-11</t>
+        </is>
+      </c>
+      <c r="Q127" t="inlineStr">
+        <is>
+          <t>DC-11</t>
+        </is>
+      </c>
+      <c r="R127" t="inlineStr">
+        <is>
+          <t>DC-11</t>
+        </is>
+      </c>
+      <c r="S127" t="inlineStr">
+        <is>
+          <t>DC-11</t>
+        </is>
+      </c>
+      <c r="T127" t="inlineStr">
+        <is>
+          <t>DC-11</t>
+        </is>
+      </c>
+      <c r="U127" t="inlineStr">
+        <is>
+          <t>DC-11</t>
+        </is>
+      </c>
+      <c r="V127" t="inlineStr">
+        <is>
+          <t>DC-11</t>
+        </is>
+      </c>
+      <c r="W127" t="inlineStr">
+        <is>
+          <t>DC-11</t>
+        </is>
+      </c>
     </row>
     <row r="128">
       <c r="A128" t="inlineStr">
@@ -4272,6 +5072,76 @@
           <t>Detalle</t>
         </is>
       </c>
+      <c r="C136" t="inlineStr">
+        <is>
+          <t>DC-11</t>
+        </is>
+      </c>
+      <c r="G136" t="inlineStr">
+        <is>
+          <t>DC-11</t>
+        </is>
+      </c>
+      <c r="H136" t="inlineStr">
+        <is>
+          <t>DC-11</t>
+        </is>
+      </c>
+      <c r="K136" t="inlineStr">
+        <is>
+          <t>DC-9</t>
+        </is>
+      </c>
+      <c r="L136" t="inlineStr">
+        <is>
+          <t>DC-9</t>
+        </is>
+      </c>
+      <c r="O136" t="inlineStr">
+        <is>
+          <t>DC-11</t>
+        </is>
+      </c>
+      <c r="P136" t="inlineStr">
+        <is>
+          <t>DC-11</t>
+        </is>
+      </c>
+      <c r="Q136" t="inlineStr">
+        <is>
+          <t>DC-11</t>
+        </is>
+      </c>
+      <c r="R136" t="inlineStr">
+        <is>
+          <t>DC-11</t>
+        </is>
+      </c>
+      <c r="S136" t="inlineStr">
+        <is>
+          <t>DC-11</t>
+        </is>
+      </c>
+      <c r="T136" t="inlineStr">
+        <is>
+          <t>DC-11</t>
+        </is>
+      </c>
+      <c r="U136" t="inlineStr">
+        <is>
+          <t>DC-11</t>
+        </is>
+      </c>
+      <c r="V136" t="inlineStr">
+        <is>
+          <t>DC-11</t>
+        </is>
+      </c>
+      <c r="W136" t="inlineStr">
+        <is>
+          <t>DC-11</t>
+        </is>
+      </c>
     </row>
     <row r="137">
       <c r="A137" t="inlineStr">
@@ -4550,6 +5420,76 @@
           <t>Detalle</t>
         </is>
       </c>
+      <c r="C145" t="inlineStr">
+        <is>
+          <t>DC-11</t>
+        </is>
+      </c>
+      <c r="G145" t="inlineStr">
+        <is>
+          <t>DC-11</t>
+        </is>
+      </c>
+      <c r="H145" t="inlineStr">
+        <is>
+          <t>DC-11</t>
+        </is>
+      </c>
+      <c r="K145" t="inlineStr">
+        <is>
+          <t>DC-9</t>
+        </is>
+      </c>
+      <c r="L145" t="inlineStr">
+        <is>
+          <t>DC-9</t>
+        </is>
+      </c>
+      <c r="O145" t="inlineStr">
+        <is>
+          <t>DC-11</t>
+        </is>
+      </c>
+      <c r="P145" t="inlineStr">
+        <is>
+          <t>DC-11</t>
+        </is>
+      </c>
+      <c r="Q145" t="inlineStr">
+        <is>
+          <t>DC-11</t>
+        </is>
+      </c>
+      <c r="R145" t="inlineStr">
+        <is>
+          <t>DC-11</t>
+        </is>
+      </c>
+      <c r="S145" t="inlineStr">
+        <is>
+          <t>DC-11</t>
+        </is>
+      </c>
+      <c r="T145" t="inlineStr">
+        <is>
+          <t>DC-11</t>
+        </is>
+      </c>
+      <c r="U145" t="inlineStr">
+        <is>
+          <t>DC-11</t>
+        </is>
+      </c>
+      <c r="V145" t="inlineStr">
+        <is>
+          <t>DC-11</t>
+        </is>
+      </c>
+      <c r="W145" t="inlineStr">
+        <is>
+          <t>DC-11</t>
+        </is>
+      </c>
     </row>
     <row r="146">
       <c r="A146" t="inlineStr">
@@ -4828,6 +5768,76 @@
           <t>Detalle</t>
         </is>
       </c>
+      <c r="C154" t="inlineStr">
+        <is>
+          <t>DC-11</t>
+        </is>
+      </c>
+      <c r="G154" t="inlineStr">
+        <is>
+          <t>DC-11</t>
+        </is>
+      </c>
+      <c r="H154" t="inlineStr">
+        <is>
+          <t>DC-11</t>
+        </is>
+      </c>
+      <c r="K154" t="inlineStr">
+        <is>
+          <t>DC-9</t>
+        </is>
+      </c>
+      <c r="L154" t="inlineStr">
+        <is>
+          <t>DC-9</t>
+        </is>
+      </c>
+      <c r="O154" t="inlineStr">
+        <is>
+          <t>DC-11</t>
+        </is>
+      </c>
+      <c r="P154" t="inlineStr">
+        <is>
+          <t>DC-11</t>
+        </is>
+      </c>
+      <c r="Q154" t="inlineStr">
+        <is>
+          <t>DC-11</t>
+        </is>
+      </c>
+      <c r="R154" t="inlineStr">
+        <is>
+          <t>DC-11</t>
+        </is>
+      </c>
+      <c r="S154" t="inlineStr">
+        <is>
+          <t>DC-11</t>
+        </is>
+      </c>
+      <c r="T154" t="inlineStr">
+        <is>
+          <t>DC-11</t>
+        </is>
+      </c>
+      <c r="U154" t="inlineStr">
+        <is>
+          <t>DC-11</t>
+        </is>
+      </c>
+      <c r="V154" t="inlineStr">
+        <is>
+          <t>DC-11</t>
+        </is>
+      </c>
+      <c r="W154" t="inlineStr">
+        <is>
+          <t>DC-11</t>
+        </is>
+      </c>
     </row>
     <row r="155">
       <c r="A155" t="inlineStr">
@@ -5106,6 +6116,76 @@
           <t>Detalle</t>
         </is>
       </c>
+      <c r="C163" t="inlineStr">
+        <is>
+          <t>DC-11</t>
+        </is>
+      </c>
+      <c r="G163" t="inlineStr">
+        <is>
+          <t>DC-11</t>
+        </is>
+      </c>
+      <c r="H163" t="inlineStr">
+        <is>
+          <t>DC-11</t>
+        </is>
+      </c>
+      <c r="K163" t="inlineStr">
+        <is>
+          <t>DC-14</t>
+        </is>
+      </c>
+      <c r="L163" t="inlineStr">
+        <is>
+          <t>DC-14</t>
+        </is>
+      </c>
+      <c r="O163" t="inlineStr">
+        <is>
+          <t>DC-11</t>
+        </is>
+      </c>
+      <c r="P163" t="inlineStr">
+        <is>
+          <t>DC-11</t>
+        </is>
+      </c>
+      <c r="Q163" t="inlineStr">
+        <is>
+          <t>DC-11</t>
+        </is>
+      </c>
+      <c r="R163" t="inlineStr">
+        <is>
+          <t>DC-11</t>
+        </is>
+      </c>
+      <c r="S163" t="inlineStr">
+        <is>
+          <t>DC-11</t>
+        </is>
+      </c>
+      <c r="T163" t="inlineStr">
+        <is>
+          <t>DC-11</t>
+        </is>
+      </c>
+      <c r="U163" t="inlineStr">
+        <is>
+          <t>DC-11</t>
+        </is>
+      </c>
+      <c r="V163" t="inlineStr">
+        <is>
+          <t>DC-11</t>
+        </is>
+      </c>
+      <c r="W163" t="inlineStr">
+        <is>
+          <t>DC-11</t>
+        </is>
+      </c>
     </row>
     <row r="164">
       <c r="A164" t="inlineStr">
@@ -5384,6 +6464,76 @@
           <t>Detalle</t>
         </is>
       </c>
+      <c r="C172" t="inlineStr">
+        <is>
+          <t>DC-11</t>
+        </is>
+      </c>
+      <c r="G172" t="inlineStr">
+        <is>
+          <t>DC-11</t>
+        </is>
+      </c>
+      <c r="H172" t="inlineStr">
+        <is>
+          <t>DC-11</t>
+        </is>
+      </c>
+      <c r="K172" t="inlineStr">
+        <is>
+          <t>DC-14</t>
+        </is>
+      </c>
+      <c r="L172" t="inlineStr">
+        <is>
+          <t>DC-14</t>
+        </is>
+      </c>
+      <c r="O172" t="inlineStr">
+        <is>
+          <t>DC-11</t>
+        </is>
+      </c>
+      <c r="P172" t="inlineStr">
+        <is>
+          <t>DC-11</t>
+        </is>
+      </c>
+      <c r="Q172" t="inlineStr">
+        <is>
+          <t>DC-11</t>
+        </is>
+      </c>
+      <c r="R172" t="inlineStr">
+        <is>
+          <t>DC-11</t>
+        </is>
+      </c>
+      <c r="S172" t="inlineStr">
+        <is>
+          <t>DC-11</t>
+        </is>
+      </c>
+      <c r="T172" t="inlineStr">
+        <is>
+          <t>DC-11</t>
+        </is>
+      </c>
+      <c r="U172" t="inlineStr">
+        <is>
+          <t>DC-11</t>
+        </is>
+      </c>
+      <c r="V172" t="inlineStr">
+        <is>
+          <t>DC-11</t>
+        </is>
+      </c>
+      <c r="W172" t="inlineStr">
+        <is>
+          <t>DC-11</t>
+        </is>
+      </c>
     </row>
     <row r="173">
       <c r="A173" t="inlineStr">
@@ -5662,6 +6812,76 @@
           <t>Detalle</t>
         </is>
       </c>
+      <c r="C181" t="inlineStr">
+        <is>
+          <t>DC-11</t>
+        </is>
+      </c>
+      <c r="G181" t="inlineStr">
+        <is>
+          <t>DC-11</t>
+        </is>
+      </c>
+      <c r="H181" t="inlineStr">
+        <is>
+          <t>DC-11</t>
+        </is>
+      </c>
+      <c r="K181" t="inlineStr">
+        <is>
+          <t>DC-14</t>
+        </is>
+      </c>
+      <c r="L181" t="inlineStr">
+        <is>
+          <t>DC-14</t>
+        </is>
+      </c>
+      <c r="O181" t="inlineStr">
+        <is>
+          <t>DC-11</t>
+        </is>
+      </c>
+      <c r="P181" t="inlineStr">
+        <is>
+          <t>DC-11</t>
+        </is>
+      </c>
+      <c r="Q181" t="inlineStr">
+        <is>
+          <t>DC-11</t>
+        </is>
+      </c>
+      <c r="R181" t="inlineStr">
+        <is>
+          <t>DC-11</t>
+        </is>
+      </c>
+      <c r="S181" t="inlineStr">
+        <is>
+          <t>DC-11</t>
+        </is>
+      </c>
+      <c r="T181" t="inlineStr">
+        <is>
+          <t>DC-11</t>
+        </is>
+      </c>
+      <c r="U181" t="inlineStr">
+        <is>
+          <t>DC-11</t>
+        </is>
+      </c>
+      <c r="V181" t="inlineStr">
+        <is>
+          <t>DC-11</t>
+        </is>
+      </c>
+      <c r="W181" t="inlineStr">
+        <is>
+          <t>DC-11</t>
+        </is>
+      </c>
     </row>
     <row r="182">
       <c r="A182" t="inlineStr">
@@ -5940,6 +7160,76 @@
           <t>Detalle</t>
         </is>
       </c>
+      <c r="C190" t="inlineStr">
+        <is>
+          <t>DC-11</t>
+        </is>
+      </c>
+      <c r="G190" t="inlineStr">
+        <is>
+          <t>DC-11</t>
+        </is>
+      </c>
+      <c r="H190" t="inlineStr">
+        <is>
+          <t>DC-11</t>
+        </is>
+      </c>
+      <c r="K190" t="inlineStr">
+        <is>
+          <t>DC-13</t>
+        </is>
+      </c>
+      <c r="L190" t="inlineStr">
+        <is>
+          <t>DC-13</t>
+        </is>
+      </c>
+      <c r="O190" t="inlineStr">
+        <is>
+          <t>DC-11</t>
+        </is>
+      </c>
+      <c r="P190" t="inlineStr">
+        <is>
+          <t>DC-11</t>
+        </is>
+      </c>
+      <c r="Q190" t="inlineStr">
+        <is>
+          <t>DC-11</t>
+        </is>
+      </c>
+      <c r="R190" t="inlineStr">
+        <is>
+          <t>DC-11</t>
+        </is>
+      </c>
+      <c r="S190" t="inlineStr">
+        <is>
+          <t>DC-11</t>
+        </is>
+      </c>
+      <c r="T190" t="inlineStr">
+        <is>
+          <t>DC-11</t>
+        </is>
+      </c>
+      <c r="U190" t="inlineStr">
+        <is>
+          <t>DC-11</t>
+        </is>
+      </c>
+      <c r="V190" t="inlineStr">
+        <is>
+          <t>DC-11</t>
+        </is>
+      </c>
+      <c r="W190" t="inlineStr">
+        <is>
+          <t>DC-11</t>
+        </is>
+      </c>
     </row>
     <row r="191">
       <c r="A191" t="inlineStr">
@@ -6218,6 +7508,76 @@
           <t>Detalle</t>
         </is>
       </c>
+      <c r="C199" t="inlineStr">
+        <is>
+          <t>DC-11</t>
+        </is>
+      </c>
+      <c r="G199" t="inlineStr">
+        <is>
+          <t>DC-11</t>
+        </is>
+      </c>
+      <c r="H199" t="inlineStr">
+        <is>
+          <t>DC-11</t>
+        </is>
+      </c>
+      <c r="K199" t="inlineStr">
+        <is>
+          <t>DC-13</t>
+        </is>
+      </c>
+      <c r="L199" t="inlineStr">
+        <is>
+          <t>DC-13</t>
+        </is>
+      </c>
+      <c r="O199" t="inlineStr">
+        <is>
+          <t>DC-11</t>
+        </is>
+      </c>
+      <c r="P199" t="inlineStr">
+        <is>
+          <t>DC-11</t>
+        </is>
+      </c>
+      <c r="Q199" t="inlineStr">
+        <is>
+          <t>DC-11</t>
+        </is>
+      </c>
+      <c r="R199" t="inlineStr">
+        <is>
+          <t>DC-11</t>
+        </is>
+      </c>
+      <c r="S199" t="inlineStr">
+        <is>
+          <t>DC-11</t>
+        </is>
+      </c>
+      <c r="T199" t="inlineStr">
+        <is>
+          <t>DC-11</t>
+        </is>
+      </c>
+      <c r="U199" t="inlineStr">
+        <is>
+          <t>DC-11</t>
+        </is>
+      </c>
+      <c r="V199" t="inlineStr">
+        <is>
+          <t>DC-11</t>
+        </is>
+      </c>
+      <c r="W199" t="inlineStr">
+        <is>
+          <t>DC-11</t>
+        </is>
+      </c>
     </row>
     <row r="200">
       <c r="A200" t="inlineStr">
@@ -6496,6 +7856,76 @@
           <t>Detalle</t>
         </is>
       </c>
+      <c r="C208" t="inlineStr">
+        <is>
+          <t>DC-11</t>
+        </is>
+      </c>
+      <c r="G208" t="inlineStr">
+        <is>
+          <t>DC-11</t>
+        </is>
+      </c>
+      <c r="H208" t="inlineStr">
+        <is>
+          <t>DC-11</t>
+        </is>
+      </c>
+      <c r="K208" t="inlineStr">
+        <is>
+          <t>DC-13</t>
+        </is>
+      </c>
+      <c r="L208" t="inlineStr">
+        <is>
+          <t>DC-13</t>
+        </is>
+      </c>
+      <c r="O208" t="inlineStr">
+        <is>
+          <t>DC-11</t>
+        </is>
+      </c>
+      <c r="P208" t="inlineStr">
+        <is>
+          <t>DC-11</t>
+        </is>
+      </c>
+      <c r="Q208" t="inlineStr">
+        <is>
+          <t>DC-11</t>
+        </is>
+      </c>
+      <c r="R208" t="inlineStr">
+        <is>
+          <t>DC-11</t>
+        </is>
+      </c>
+      <c r="S208" t="inlineStr">
+        <is>
+          <t>DC-11</t>
+        </is>
+      </c>
+      <c r="T208" t="inlineStr">
+        <is>
+          <t>DC-11</t>
+        </is>
+      </c>
+      <c r="U208" t="inlineStr">
+        <is>
+          <t>DC-11</t>
+        </is>
+      </c>
+      <c r="V208" t="inlineStr">
+        <is>
+          <t>DC-11</t>
+        </is>
+      </c>
+      <c r="W208" t="inlineStr">
+        <is>
+          <t>DC-11</t>
+        </is>
+      </c>
     </row>
     <row r="209">
       <c r="A209" t="inlineStr">
@@ -6774,6 +8204,76 @@
           <t>Detalle</t>
         </is>
       </c>
+      <c r="C217" t="inlineStr">
+        <is>
+          <t>DC-11</t>
+        </is>
+      </c>
+      <c r="G217" t="inlineStr">
+        <is>
+          <t>DC-11</t>
+        </is>
+      </c>
+      <c r="H217" t="inlineStr">
+        <is>
+          <t>DC-10</t>
+        </is>
+      </c>
+      <c r="K217" t="inlineStr">
+        <is>
+          <t>DC-12</t>
+        </is>
+      </c>
+      <c r="L217" t="inlineStr">
+        <is>
+          <t>DC-12</t>
+        </is>
+      </c>
+      <c r="O217" t="inlineStr">
+        <is>
+          <t>DC-10</t>
+        </is>
+      </c>
+      <c r="P217" t="inlineStr">
+        <is>
+          <t>DC-11</t>
+        </is>
+      </c>
+      <c r="Q217" t="inlineStr">
+        <is>
+          <t>DC-11</t>
+        </is>
+      </c>
+      <c r="R217" t="inlineStr">
+        <is>
+          <t>DC-11</t>
+        </is>
+      </c>
+      <c r="S217" t="inlineStr">
+        <is>
+          <t>DC-11</t>
+        </is>
+      </c>
+      <c r="T217" t="inlineStr">
+        <is>
+          <t>DC-11</t>
+        </is>
+      </c>
+      <c r="U217" t="inlineStr">
+        <is>
+          <t>DC-11</t>
+        </is>
+      </c>
+      <c r="V217" t="inlineStr">
+        <is>
+          <t>DC-11</t>
+        </is>
+      </c>
+      <c r="W217" t="inlineStr">
+        <is>
+          <t>DC-11</t>
+        </is>
+      </c>
     </row>
     <row r="218">
       <c r="A218" t="inlineStr">
@@ -7052,6 +8552,76 @@
           <t>Detalle</t>
         </is>
       </c>
+      <c r="C226" t="inlineStr">
+        <is>
+          <t>DC-11</t>
+        </is>
+      </c>
+      <c r="G226" t="inlineStr">
+        <is>
+          <t>DC-11</t>
+        </is>
+      </c>
+      <c r="H226" t="inlineStr">
+        <is>
+          <t>DC-10</t>
+        </is>
+      </c>
+      <c r="K226" t="inlineStr">
+        <is>
+          <t>DC-12</t>
+        </is>
+      </c>
+      <c r="L226" t="inlineStr">
+        <is>
+          <t>DC-12</t>
+        </is>
+      </c>
+      <c r="O226" t="inlineStr">
+        <is>
+          <t>DC-10</t>
+        </is>
+      </c>
+      <c r="P226" t="inlineStr">
+        <is>
+          <t>DC-11</t>
+        </is>
+      </c>
+      <c r="Q226" t="inlineStr">
+        <is>
+          <t>DC-11</t>
+        </is>
+      </c>
+      <c r="R226" t="inlineStr">
+        <is>
+          <t>DC-11</t>
+        </is>
+      </c>
+      <c r="S226" t="inlineStr">
+        <is>
+          <t>DC-11</t>
+        </is>
+      </c>
+      <c r="T226" t="inlineStr">
+        <is>
+          <t>DC-11</t>
+        </is>
+      </c>
+      <c r="U226" t="inlineStr">
+        <is>
+          <t>DC-11</t>
+        </is>
+      </c>
+      <c r="V226" t="inlineStr">
+        <is>
+          <t>DC-11</t>
+        </is>
+      </c>
+      <c r="W226" t="inlineStr">
+        <is>
+          <t>DC-11</t>
+        </is>
+      </c>
     </row>
     <row r="227">
       <c r="A227" t="inlineStr">
@@ -7330,6 +8900,76 @@
           <t>Detalle</t>
         </is>
       </c>
+      <c r="C235" t="inlineStr">
+        <is>
+          <t>DC-11</t>
+        </is>
+      </c>
+      <c r="G235" t="inlineStr">
+        <is>
+          <t>DC-11</t>
+        </is>
+      </c>
+      <c r="H235" t="inlineStr">
+        <is>
+          <t>DC-10</t>
+        </is>
+      </c>
+      <c r="K235" t="inlineStr">
+        <is>
+          <t>DC-12</t>
+        </is>
+      </c>
+      <c r="L235" t="inlineStr">
+        <is>
+          <t>DC-12</t>
+        </is>
+      </c>
+      <c r="O235" t="inlineStr">
+        <is>
+          <t>DC-10</t>
+        </is>
+      </c>
+      <c r="P235" t="inlineStr">
+        <is>
+          <t>DC-11</t>
+        </is>
+      </c>
+      <c r="Q235" t="inlineStr">
+        <is>
+          <t>DC-11</t>
+        </is>
+      </c>
+      <c r="R235" t="inlineStr">
+        <is>
+          <t>DC-11</t>
+        </is>
+      </c>
+      <c r="S235" t="inlineStr">
+        <is>
+          <t>DC-11</t>
+        </is>
+      </c>
+      <c r="T235" t="inlineStr">
+        <is>
+          <t>DC-11</t>
+        </is>
+      </c>
+      <c r="U235" t="inlineStr">
+        <is>
+          <t>DC-11</t>
+        </is>
+      </c>
+      <c r="V235" t="inlineStr">
+        <is>
+          <t>DC-11</t>
+        </is>
+      </c>
+      <c r="W235" t="inlineStr">
+        <is>
+          <t>DC-11</t>
+        </is>
+      </c>
     </row>
     <row r="236">
       <c r="A236" t="inlineStr">
@@ -7938,6 +9578,186 @@
           <t>Detalle</t>
         </is>
       </c>
+      <c r="C244" t="inlineStr">
+        <is>
+          <t>DC-3</t>
+        </is>
+      </c>
+      <c r="D244" t="inlineStr">
+        <is>
+          <t>DC-2</t>
+        </is>
+      </c>
+      <c r="E244" t="inlineStr">
+        <is>
+          <t>DC-2</t>
+        </is>
+      </c>
+      <c r="F244" t="inlineStr">
+        <is>
+          <t>DC-2</t>
+        </is>
+      </c>
+      <c r="G244" t="inlineStr">
+        <is>
+          <t>DC-3</t>
+        </is>
+      </c>
+      <c r="H244" t="inlineStr">
+        <is>
+          <t>DC-4</t>
+        </is>
+      </c>
+      <c r="I244" t="inlineStr">
+        <is>
+          <t>DC-5</t>
+        </is>
+      </c>
+      <c r="J244" t="inlineStr">
+        <is>
+          <t>DC-5</t>
+        </is>
+      </c>
+      <c r="K244" t="inlineStr">
+        <is>
+          <t>DC-6</t>
+        </is>
+      </c>
+      <c r="L244" t="inlineStr">
+        <is>
+          <t>DC-6</t>
+        </is>
+      </c>
+      <c r="M244" t="inlineStr">
+        <is>
+          <t>DC-5</t>
+        </is>
+      </c>
+      <c r="N244" t="inlineStr">
+        <is>
+          <t>DC-5</t>
+        </is>
+      </c>
+      <c r="O244" t="inlineStr">
+        <is>
+          <t>DC-4</t>
+        </is>
+      </c>
+      <c r="P244" t="inlineStr">
+        <is>
+          <t>DC-3</t>
+        </is>
+      </c>
+      <c r="Q244" t="inlineStr">
+        <is>
+          <t>DC-3</t>
+        </is>
+      </c>
+      <c r="R244" t="inlineStr">
+        <is>
+          <t>DC-3</t>
+        </is>
+      </c>
+      <c r="S244" t="inlineStr">
+        <is>
+          <t>DC-3</t>
+        </is>
+      </c>
+      <c r="T244" t="inlineStr">
+        <is>
+          <t>DC-3</t>
+        </is>
+      </c>
+      <c r="U244" t="inlineStr">
+        <is>
+          <t>DC-3</t>
+        </is>
+      </c>
+      <c r="V244" t="inlineStr">
+        <is>
+          <t>DC-3</t>
+        </is>
+      </c>
+      <c r="W244" t="inlineStr">
+        <is>
+          <t>DC-3</t>
+        </is>
+      </c>
+      <c r="AB244" t="inlineStr">
+        <is>
+          <t>DC-5</t>
+        </is>
+      </c>
+      <c r="AC244" t="inlineStr">
+        <is>
+          <t>DC-5</t>
+        </is>
+      </c>
+      <c r="AD244" t="inlineStr">
+        <is>
+          <t>DC-5</t>
+        </is>
+      </c>
+      <c r="AE244" t="inlineStr">
+        <is>
+          <t>DC-5</t>
+        </is>
+      </c>
+      <c r="AF244" t="inlineStr">
+        <is>
+          <t>DC-2</t>
+        </is>
+      </c>
+      <c r="AG244" t="inlineStr">
+        <is>
+          <t>DC-2</t>
+        </is>
+      </c>
+      <c r="AH244" t="inlineStr">
+        <is>
+          <t>DC-2</t>
+        </is>
+      </c>
+      <c r="AI244" t="inlineStr">
+        <is>
+          <t>DC-2</t>
+        </is>
+      </c>
+      <c r="AJ244" t="inlineStr">
+        <is>
+          <t>DC-8</t>
+        </is>
+      </c>
+      <c r="AL244" t="inlineStr">
+        <is>
+          <t>DC-2</t>
+        </is>
+      </c>
+      <c r="AM244" t="inlineStr">
+        <is>
+          <t>DC-2</t>
+        </is>
+      </c>
+      <c r="AN244" t="inlineStr">
+        <is>
+          <t>DC-2</t>
+        </is>
+      </c>
+      <c r="AO244" t="inlineStr">
+        <is>
+          <t>DC-2</t>
+        </is>
+      </c>
+      <c r="AP244" t="inlineStr">
+        <is>
+          <t>DC-2</t>
+        </is>
+      </c>
+      <c r="AQ244" t="inlineStr">
+        <is>
+          <t>DC-2</t>
+        </is>
+      </c>
     </row>
     <row r="245">
       <c r="A245" t="inlineStr">
@@ -8426,6 +10246,146 @@
           <t>Detalle</t>
         </is>
       </c>
+      <c r="C253" t="inlineStr">
+        <is>
+          <t>DC-3</t>
+        </is>
+      </c>
+      <c r="D253" t="inlineStr">
+        <is>
+          <t>DC-2</t>
+        </is>
+      </c>
+      <c r="E253" t="inlineStr">
+        <is>
+          <t>DC-2</t>
+        </is>
+      </c>
+      <c r="F253" t="inlineStr">
+        <is>
+          <t>DC-2</t>
+        </is>
+      </c>
+      <c r="G253" t="inlineStr">
+        <is>
+          <t>DC-3</t>
+        </is>
+      </c>
+      <c r="H253" t="inlineStr">
+        <is>
+          <t>DC-4</t>
+        </is>
+      </c>
+      <c r="I253" t="inlineStr">
+        <is>
+          <t>DC-5</t>
+        </is>
+      </c>
+      <c r="J253" t="inlineStr">
+        <is>
+          <t>DC-5</t>
+        </is>
+      </c>
+      <c r="L253" t="inlineStr">
+        <is>
+          <t>DC-6</t>
+        </is>
+      </c>
+      <c r="M253" t="inlineStr">
+        <is>
+          <t>DC-5</t>
+        </is>
+      </c>
+      <c r="N253" t="inlineStr">
+        <is>
+          <t>DC-5</t>
+        </is>
+      </c>
+      <c r="O253" t="inlineStr">
+        <is>
+          <t>DC-4</t>
+        </is>
+      </c>
+      <c r="P253" t="inlineStr">
+        <is>
+          <t>DC-3</t>
+        </is>
+      </c>
+      <c r="Q253" t="inlineStr">
+        <is>
+          <t>DC-3</t>
+        </is>
+      </c>
+      <c r="R253" t="inlineStr">
+        <is>
+          <t>DC-3</t>
+        </is>
+      </c>
+      <c r="S253" t="inlineStr">
+        <is>
+          <t>DC-3</t>
+        </is>
+      </c>
+      <c r="U253" t="inlineStr">
+        <is>
+          <t>DC-3</t>
+        </is>
+      </c>
+      <c r="V253" t="inlineStr">
+        <is>
+          <t>DC-3</t>
+        </is>
+      </c>
+      <c r="W253" t="inlineStr">
+        <is>
+          <t>DC-3</t>
+        </is>
+      </c>
+      <c r="AF253" t="inlineStr">
+        <is>
+          <t>DC-2</t>
+        </is>
+      </c>
+      <c r="AG253" t="inlineStr">
+        <is>
+          <t>DC-2</t>
+        </is>
+      </c>
+      <c r="AH253" t="inlineStr">
+        <is>
+          <t>DC-2</t>
+        </is>
+      </c>
+      <c r="AI253" t="inlineStr">
+        <is>
+          <t>DC-2</t>
+        </is>
+      </c>
+      <c r="AJ253" t="inlineStr">
+        <is>
+          <t>DC-8</t>
+        </is>
+      </c>
+      <c r="AL253" t="inlineStr">
+        <is>
+          <t>DC-2</t>
+        </is>
+      </c>
+      <c r="AM253" t="inlineStr">
+        <is>
+          <t>DC-2</t>
+        </is>
+      </c>
+      <c r="AN253" t="inlineStr">
+        <is>
+          <t>DC-2</t>
+        </is>
+      </c>
+      <c r="AO253" t="inlineStr">
+        <is>
+          <t>DC-2</t>
+        </is>
+      </c>
     </row>
     <row r="254">
       <c r="A254" t="inlineStr">
@@ -8914,6 +10874,146 @@
           <t>Detalle</t>
         </is>
       </c>
+      <c r="C262" t="inlineStr">
+        <is>
+          <t>DC-3</t>
+        </is>
+      </c>
+      <c r="D262" t="inlineStr">
+        <is>
+          <t>DC-2</t>
+        </is>
+      </c>
+      <c r="E262" t="inlineStr">
+        <is>
+          <t>DC-2</t>
+        </is>
+      </c>
+      <c r="F262" t="inlineStr">
+        <is>
+          <t>DC-2</t>
+        </is>
+      </c>
+      <c r="G262" t="inlineStr">
+        <is>
+          <t>DC-3</t>
+        </is>
+      </c>
+      <c r="H262" t="inlineStr">
+        <is>
+          <t>DC-4</t>
+        </is>
+      </c>
+      <c r="I262" t="inlineStr">
+        <is>
+          <t>DC-5</t>
+        </is>
+      </c>
+      <c r="J262" t="inlineStr">
+        <is>
+          <t>DC-5</t>
+        </is>
+      </c>
+      <c r="L262" t="inlineStr">
+        <is>
+          <t>DC-6</t>
+        </is>
+      </c>
+      <c r="M262" t="inlineStr">
+        <is>
+          <t>DC-5</t>
+        </is>
+      </c>
+      <c r="N262" t="inlineStr">
+        <is>
+          <t>DC-5</t>
+        </is>
+      </c>
+      <c r="O262" t="inlineStr">
+        <is>
+          <t>DC-4</t>
+        </is>
+      </c>
+      <c r="P262" t="inlineStr">
+        <is>
+          <t>DC-3</t>
+        </is>
+      </c>
+      <c r="Q262" t="inlineStr">
+        <is>
+          <t>DC-3</t>
+        </is>
+      </c>
+      <c r="R262" t="inlineStr">
+        <is>
+          <t>DC-3</t>
+        </is>
+      </c>
+      <c r="S262" t="inlineStr">
+        <is>
+          <t>DC-3</t>
+        </is>
+      </c>
+      <c r="U262" t="inlineStr">
+        <is>
+          <t>DC-3</t>
+        </is>
+      </c>
+      <c r="V262" t="inlineStr">
+        <is>
+          <t>DC-3</t>
+        </is>
+      </c>
+      <c r="W262" t="inlineStr">
+        <is>
+          <t>DC-3</t>
+        </is>
+      </c>
+      <c r="AF262" t="inlineStr">
+        <is>
+          <t>DC-2</t>
+        </is>
+      </c>
+      <c r="AG262" t="inlineStr">
+        <is>
+          <t>DC-2</t>
+        </is>
+      </c>
+      <c r="AH262" t="inlineStr">
+        <is>
+          <t>DC-2</t>
+        </is>
+      </c>
+      <c r="AI262" t="inlineStr">
+        <is>
+          <t>DC-2</t>
+        </is>
+      </c>
+      <c r="AJ262" t="inlineStr">
+        <is>
+          <t>DC-8</t>
+        </is>
+      </c>
+      <c r="AL262" t="inlineStr">
+        <is>
+          <t>DC-2</t>
+        </is>
+      </c>
+      <c r="AM262" t="inlineStr">
+        <is>
+          <t>DC-2</t>
+        </is>
+      </c>
+      <c r="AN262" t="inlineStr">
+        <is>
+          <t>DC-2</t>
+        </is>
+      </c>
+      <c r="AO262" t="inlineStr">
+        <is>
+          <t>DC-2</t>
+        </is>
+      </c>
     </row>
     <row r="263">
       <c r="A263" t="inlineStr">
@@ -9402,6 +11502,146 @@
           <t>Detalle</t>
         </is>
       </c>
+      <c r="C271" t="inlineStr">
+        <is>
+          <t>DC-1</t>
+        </is>
+      </c>
+      <c r="D271" t="inlineStr">
+        <is>
+          <t>DC-2</t>
+        </is>
+      </c>
+      <c r="E271" t="inlineStr">
+        <is>
+          <t>DC-2</t>
+        </is>
+      </c>
+      <c r="F271" t="inlineStr">
+        <is>
+          <t>DC-2</t>
+        </is>
+      </c>
+      <c r="G271" t="inlineStr">
+        <is>
+          <t>DC-3</t>
+        </is>
+      </c>
+      <c r="H271" t="inlineStr">
+        <is>
+          <t>DC-4</t>
+        </is>
+      </c>
+      <c r="I271" t="inlineStr">
+        <is>
+          <t>DC-5</t>
+        </is>
+      </c>
+      <c r="J271" t="inlineStr">
+        <is>
+          <t>DC-5</t>
+        </is>
+      </c>
+      <c r="L271" t="inlineStr">
+        <is>
+          <t>DC-6</t>
+        </is>
+      </c>
+      <c r="M271" t="inlineStr">
+        <is>
+          <t>DC-5</t>
+        </is>
+      </c>
+      <c r="N271" t="inlineStr">
+        <is>
+          <t>DC-5</t>
+        </is>
+      </c>
+      <c r="O271" t="inlineStr">
+        <is>
+          <t>DC-4</t>
+        </is>
+      </c>
+      <c r="P271" t="inlineStr">
+        <is>
+          <t>DC-3</t>
+        </is>
+      </c>
+      <c r="Q271" t="inlineStr">
+        <is>
+          <t>DC-7</t>
+        </is>
+      </c>
+      <c r="R271" t="inlineStr">
+        <is>
+          <t>DC-7</t>
+        </is>
+      </c>
+      <c r="S271" t="inlineStr">
+        <is>
+          <t>DC-7</t>
+        </is>
+      </c>
+      <c r="U271" t="inlineStr">
+        <is>
+          <t>DC-7</t>
+        </is>
+      </c>
+      <c r="V271" t="inlineStr">
+        <is>
+          <t>DC-7</t>
+        </is>
+      </c>
+      <c r="W271" t="inlineStr">
+        <is>
+          <t>DC-3</t>
+        </is>
+      </c>
+      <c r="AF271" t="inlineStr">
+        <is>
+          <t>DC-2</t>
+        </is>
+      </c>
+      <c r="AG271" t="inlineStr">
+        <is>
+          <t>DC-2</t>
+        </is>
+      </c>
+      <c r="AH271" t="inlineStr">
+        <is>
+          <t>DC-2</t>
+        </is>
+      </c>
+      <c r="AI271" t="inlineStr">
+        <is>
+          <t>DC-2</t>
+        </is>
+      </c>
+      <c r="AJ271" t="inlineStr">
+        <is>
+          <t>DC-8</t>
+        </is>
+      </c>
+      <c r="AL271" t="inlineStr">
+        <is>
+          <t>DC-2</t>
+        </is>
+      </c>
+      <c r="AM271" t="inlineStr">
+        <is>
+          <t>DC-2</t>
+        </is>
+      </c>
+      <c r="AN271" t="inlineStr">
+        <is>
+          <t>DC-2</t>
+        </is>
+      </c>
+      <c r="AO271" t="inlineStr">
+        <is>
+          <t>DC-2</t>
+        </is>
+      </c>
     </row>
     <row r="272">
       <c r="A272" t="inlineStr">
@@ -9905,6 +12145,151 @@
           <t>Detalle</t>
         </is>
       </c>
+      <c r="C280" t="inlineStr">
+        <is>
+          <t>DC-1</t>
+        </is>
+      </c>
+      <c r="D280" t="inlineStr">
+        <is>
+          <t>DC-2</t>
+        </is>
+      </c>
+      <c r="E280" t="inlineStr">
+        <is>
+          <t>DC-2</t>
+        </is>
+      </c>
+      <c r="F280" t="inlineStr">
+        <is>
+          <t>DC-2</t>
+        </is>
+      </c>
+      <c r="G280" t="inlineStr">
+        <is>
+          <t>DC-3</t>
+        </is>
+      </c>
+      <c r="H280" t="inlineStr">
+        <is>
+          <t>DC-4</t>
+        </is>
+      </c>
+      <c r="I280" t="inlineStr">
+        <is>
+          <t>DC-5</t>
+        </is>
+      </c>
+      <c r="J280" t="inlineStr">
+        <is>
+          <t>DC-5</t>
+        </is>
+      </c>
+      <c r="L280" t="inlineStr">
+        <is>
+          <t>DC-6</t>
+        </is>
+      </c>
+      <c r="M280" t="inlineStr">
+        <is>
+          <t>DC-5</t>
+        </is>
+      </c>
+      <c r="N280" t="inlineStr">
+        <is>
+          <t>DC-5</t>
+        </is>
+      </c>
+      <c r="O280" t="inlineStr">
+        <is>
+          <t>DC-4</t>
+        </is>
+      </c>
+      <c r="P280" t="inlineStr">
+        <is>
+          <t>DC-3</t>
+        </is>
+      </c>
+      <c r="Q280" t="inlineStr">
+        <is>
+          <t>DC-7</t>
+        </is>
+      </c>
+      <c r="R280" t="inlineStr">
+        <is>
+          <t>DC-7</t>
+        </is>
+      </c>
+      <c r="S280" t="inlineStr">
+        <is>
+          <t>DC-7</t>
+        </is>
+      </c>
+      <c r="U280" t="inlineStr">
+        <is>
+          <t>DC-7</t>
+        </is>
+      </c>
+      <c r="V280" t="inlineStr">
+        <is>
+          <t>DC-7</t>
+        </is>
+      </c>
+      <c r="W280" t="inlineStr">
+        <is>
+          <t>DC-3</t>
+        </is>
+      </c>
+      <c r="Y280" t="inlineStr">
+        <is>
+          <t>DC-5</t>
+        </is>
+      </c>
+      <c r="AF280" t="inlineStr">
+        <is>
+          <t>DC-2</t>
+        </is>
+      </c>
+      <c r="AG280" t="inlineStr">
+        <is>
+          <t>DC-2</t>
+        </is>
+      </c>
+      <c r="AH280" t="inlineStr">
+        <is>
+          <t>DC-2</t>
+        </is>
+      </c>
+      <c r="AI280" t="inlineStr">
+        <is>
+          <t>DC-2</t>
+        </is>
+      </c>
+      <c r="AJ280" t="inlineStr">
+        <is>
+          <t>DC-8</t>
+        </is>
+      </c>
+      <c r="AL280" t="inlineStr">
+        <is>
+          <t>DC-2</t>
+        </is>
+      </c>
+      <c r="AM280" t="inlineStr">
+        <is>
+          <t>DC-2</t>
+        </is>
+      </c>
+      <c r="AN280" t="inlineStr">
+        <is>
+          <t>DC-2</t>
+        </is>
+      </c>
+      <c r="AO280" t="inlineStr">
+        <is>
+          <t>DC-2</t>
+        </is>
+      </c>
     </row>
     <row r="281">
       <c r="A281" t="inlineStr">
@@ -10393,6 +12778,146 @@
           <t>Detalle</t>
         </is>
       </c>
+      <c r="C289" t="inlineStr">
+        <is>
+          <t>DC-1</t>
+        </is>
+      </c>
+      <c r="D289" t="inlineStr">
+        <is>
+          <t>DC-2</t>
+        </is>
+      </c>
+      <c r="E289" t="inlineStr">
+        <is>
+          <t>DC-2</t>
+        </is>
+      </c>
+      <c r="F289" t="inlineStr">
+        <is>
+          <t>DC-2</t>
+        </is>
+      </c>
+      <c r="G289" t="inlineStr">
+        <is>
+          <t>DC-3</t>
+        </is>
+      </c>
+      <c r="H289" t="inlineStr">
+        <is>
+          <t>DC-4</t>
+        </is>
+      </c>
+      <c r="I289" t="inlineStr">
+        <is>
+          <t>DC-5</t>
+        </is>
+      </c>
+      <c r="J289" t="inlineStr">
+        <is>
+          <t>DC-5</t>
+        </is>
+      </c>
+      <c r="L289" t="inlineStr">
+        <is>
+          <t>DC-6</t>
+        </is>
+      </c>
+      <c r="M289" t="inlineStr">
+        <is>
+          <t>DC-5</t>
+        </is>
+      </c>
+      <c r="N289" t="inlineStr">
+        <is>
+          <t>DC-5</t>
+        </is>
+      </c>
+      <c r="O289" t="inlineStr">
+        <is>
+          <t>DC-4</t>
+        </is>
+      </c>
+      <c r="P289" t="inlineStr">
+        <is>
+          <t>DC-3</t>
+        </is>
+      </c>
+      <c r="Q289" t="inlineStr">
+        <is>
+          <t>DC-7</t>
+        </is>
+      </c>
+      <c r="R289" t="inlineStr">
+        <is>
+          <t>DC-7</t>
+        </is>
+      </c>
+      <c r="S289" t="inlineStr">
+        <is>
+          <t>DC-7</t>
+        </is>
+      </c>
+      <c r="U289" t="inlineStr">
+        <is>
+          <t>DC-7</t>
+        </is>
+      </c>
+      <c r="V289" t="inlineStr">
+        <is>
+          <t>DC-7</t>
+        </is>
+      </c>
+      <c r="W289" t="inlineStr">
+        <is>
+          <t>DC-3</t>
+        </is>
+      </c>
+      <c r="AF289" t="inlineStr">
+        <is>
+          <t>DC-2</t>
+        </is>
+      </c>
+      <c r="AG289" t="inlineStr">
+        <is>
+          <t>DC-2</t>
+        </is>
+      </c>
+      <c r="AH289" t="inlineStr">
+        <is>
+          <t>DC-2</t>
+        </is>
+      </c>
+      <c r="AI289" t="inlineStr">
+        <is>
+          <t>DC-2</t>
+        </is>
+      </c>
+      <c r="AJ289" t="inlineStr">
+        <is>
+          <t>DC-8</t>
+        </is>
+      </c>
+      <c r="AL289" t="inlineStr">
+        <is>
+          <t>DC-2</t>
+        </is>
+      </c>
+      <c r="AM289" t="inlineStr">
+        <is>
+          <t>DC-2</t>
+        </is>
+      </c>
+      <c r="AN289" t="inlineStr">
+        <is>
+          <t>DC-2</t>
+        </is>
+      </c>
+      <c r="AO289" t="inlineStr">
+        <is>
+          <t>DC-2</t>
+        </is>
+      </c>
     </row>
     <row r="290">
       <c r="A290" t="inlineStr">
@@ -10956,6 +13481,171 @@
           <t>Detalle</t>
         </is>
       </c>
+      <c r="C298" t="inlineStr">
+        <is>
+          <t>DC-1</t>
+        </is>
+      </c>
+      <c r="D298" t="inlineStr">
+        <is>
+          <t>DC-2</t>
+        </is>
+      </c>
+      <c r="E298" t="inlineStr">
+        <is>
+          <t>DC-2</t>
+        </is>
+      </c>
+      <c r="F298" t="inlineStr">
+        <is>
+          <t>DC-2</t>
+        </is>
+      </c>
+      <c r="G298" t="inlineStr">
+        <is>
+          <t>DC-3</t>
+        </is>
+      </c>
+      <c r="H298" t="inlineStr">
+        <is>
+          <t>DC-4</t>
+        </is>
+      </c>
+      <c r="I298" t="inlineStr">
+        <is>
+          <t>DC-5</t>
+        </is>
+      </c>
+      <c r="J298" t="inlineStr">
+        <is>
+          <t>DC-5</t>
+        </is>
+      </c>
+      <c r="K298" t="inlineStr">
+        <is>
+          <t>DC-6</t>
+        </is>
+      </c>
+      <c r="L298" t="inlineStr">
+        <is>
+          <t>DC-6</t>
+        </is>
+      </c>
+      <c r="M298" t="inlineStr">
+        <is>
+          <t>DC-5</t>
+        </is>
+      </c>
+      <c r="N298" t="inlineStr">
+        <is>
+          <t>DC-5</t>
+        </is>
+      </c>
+      <c r="O298" t="inlineStr">
+        <is>
+          <t>DC-4</t>
+        </is>
+      </c>
+      <c r="P298" t="inlineStr">
+        <is>
+          <t>DC-3</t>
+        </is>
+      </c>
+      <c r="Q298" t="inlineStr">
+        <is>
+          <t>DC-7</t>
+        </is>
+      </c>
+      <c r="R298" t="inlineStr">
+        <is>
+          <t>DC-7</t>
+        </is>
+      </c>
+      <c r="S298" t="inlineStr">
+        <is>
+          <t>DC-7</t>
+        </is>
+      </c>
+      <c r="T298" t="inlineStr">
+        <is>
+          <t>DC-3</t>
+        </is>
+      </c>
+      <c r="U298" t="inlineStr">
+        <is>
+          <t>DC-7</t>
+        </is>
+      </c>
+      <c r="V298" t="inlineStr">
+        <is>
+          <t>DC-7</t>
+        </is>
+      </c>
+      <c r="W298" t="inlineStr">
+        <is>
+          <t>DC-3</t>
+        </is>
+      </c>
+      <c r="AF298" t="inlineStr">
+        <is>
+          <t>DC-2</t>
+        </is>
+      </c>
+      <c r="AG298" t="inlineStr">
+        <is>
+          <t>DC-2</t>
+        </is>
+      </c>
+      <c r="AH298" t="inlineStr">
+        <is>
+          <t>DC-2</t>
+        </is>
+      </c>
+      <c r="AI298" t="inlineStr">
+        <is>
+          <t>DC-2</t>
+        </is>
+      </c>
+      <c r="AJ298" t="inlineStr">
+        <is>
+          <t>DC-8</t>
+        </is>
+      </c>
+      <c r="AK298" t="inlineStr">
+        <is>
+          <t>DC-2</t>
+        </is>
+      </c>
+      <c r="AL298" t="inlineStr">
+        <is>
+          <t>DC-2</t>
+        </is>
+      </c>
+      <c r="AM298" t="inlineStr">
+        <is>
+          <t>DC-2</t>
+        </is>
+      </c>
+      <c r="AN298" t="inlineStr">
+        <is>
+          <t>DC-2</t>
+        </is>
+      </c>
+      <c r="AO298" t="inlineStr">
+        <is>
+          <t>DC-2</t>
+        </is>
+      </c>
+      <c r="AP298" t="inlineStr">
+        <is>
+          <t>DC-2</t>
+        </is>
+      </c>
+      <c r="AQ298" t="inlineStr">
+        <is>
+          <t>DC-2</t>
+        </is>
+      </c>
     </row>
     <row r="299">
       <c r="A299" t="inlineStr">
@@ -11142,6 +13832,46 @@
       <c r="B307" t="inlineStr">
         <is>
           <t>Detalle</t>
+        </is>
+      </c>
+      <c r="C307" t="inlineStr">
+        <is>
+          <t>DC-1</t>
+        </is>
+      </c>
+      <c r="D307" t="inlineStr">
+        <is>
+          <t>DC-2</t>
+        </is>
+      </c>
+      <c r="E307" t="inlineStr">
+        <is>
+          <t>DC-2</t>
+        </is>
+      </c>
+      <c r="F307" t="inlineStr">
+        <is>
+          <t>DC-2</t>
+        </is>
+      </c>
+      <c r="G307" t="inlineStr">
+        <is>
+          <t>DC-3</t>
+        </is>
+      </c>
+      <c r="H307" t="inlineStr">
+        <is>
+          <t>DC-4</t>
+        </is>
+      </c>
+      <c r="I307" t="inlineStr">
+        <is>
+          <t>DC-5</t>
+        </is>
+      </c>
+      <c r="J307" t="inlineStr">
+        <is>
+          <t>DC-5</t>
         </is>
       </c>
     </row>

</xml_diff>